<commit_message>
cg: updated TAS GEC form
</commit_message>
<xml_diff>
--- a/LF/TAS/DRC/cd_lf_tas_5_resultats_gec_202209_v1.xlsx
+++ b/LF/TAS/DRC/cd_lf_tas_5_resultats_gec_202209_v1.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="96">
   <si>
     <t>type</t>
   </si>
@@ -168,16 +168,19 @@
     <t>Format: 4 chiffres (le code du site) suivis de 3 chiffres (le numéro d'ordre du répondant), séparés par un tiret. Sous la forme: XXXX-XXX</t>
   </si>
   <si>
-    <t>note</t>
-  </si>
-  <si>
-    <t>r_note2</t>
-  </si>
-  <si>
-    <t>Kato Katz results</t>
-  </si>
-  <si>
-    <t>Résultats Kato Katz</t>
+    <t>select_one yesNo</t>
+  </si>
+  <si>
+    <t>r_gec</t>
+  </si>
+  <si>
+    <t>Day and night GEC performed?</t>
+  </si>
+  <si>
+    <t>La GEC (Goutte Epaisse Calibrée) diurne et nocturne a t-elle été effectuée?</t>
+  </si>
+  <si>
+    <t>integer</t>
   </si>
   <si>
     <t>r_result_gec</t>
@@ -189,6 +192,9 @@
     <t>Resultat GEC</t>
   </si>
   <si>
+    <t>${r_gec} = 'Oui'</t>
+  </si>
+  <si>
     <t>text</t>
   </si>
   <si>
@@ -291,10 +297,10 @@
     <t>default_language</t>
   </si>
   <si>
-    <t>(Octobre 2022) RDC TAS FL - 5. Formulaire Résultat GEC V3</t>
-  </si>
-  <si>
-    <t>cd_lf_tas_5_resultats_gec_202209_v3</t>
+    <t>(Octobre 2022) RDC TAS FL - 5. Formulaire Résultat GEC V3.1</t>
+  </si>
+  <si>
+    <t>cd_lf_tas_5_resultats_gec_202209_v3_1</t>
   </si>
   <si>
     <t>French</t>
@@ -307,8 +313,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -368,6 +374,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -383,6 +396,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -391,6 +411,82 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -399,14 +495,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -421,96 +517,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="38">
     <fill>
@@ -551,13 +557,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -569,174 +635,114 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -872,19 +878,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0" tint="-0.499984740745262"/>
       </left>
@@ -903,30 +896,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -957,11 +926,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -980,156 +955,174 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1204,16 +1197,19 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1246,11 +1242,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1269,12 +1271,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1626,12 +1622,12 @@
   <sheetPr/>
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I7" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A15" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -1715,46 +1711,46 @@
       <c r="D2" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43" t="s">
+      <c r="G2" s="44"/>
+      <c r="H2" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="53" t="s">
+      <c r="I2" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="J2" s="42" t="s">
+      <c r="J2" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43" t="s">
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44" t="s">
         <v>25</v>
       </c>
-      <c r="N2" s="43"/>
-      <c r="O2" s="43"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
     </row>
     <row r="3" s="20" customFormat="1" spans="1:15">
       <c r="A3" s="23"/>
       <c r="B3" s="24"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
-      <c r="E3" s="41"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="36"/>
-      <c r="H3" s="36"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="44"/>
-      <c r="K3" s="36"/>
-      <c r="L3" s="36"/>
-      <c r="M3" s="36"/>
-      <c r="N3" s="43"/>
-      <c r="O3" s="36"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="45"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="38"/>
+      <c r="J3" s="45"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="37"/>
+      <c r="N3" s="44"/>
+      <c r="O3" s="37"/>
     </row>
     <row r="4" s="13" customFormat="1" spans="1:15">
       <c r="A4" s="23" t="s">
@@ -1769,20 +1765,20 @@
       <c r="D4" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="41"/>
+      <c r="F4" s="42"/>
       <c r="G4" s="23"/>
-      <c r="H4" s="45"/>
+      <c r="H4" s="46"/>
       <c r="I4" s="25"/>
-      <c r="J4" s="41"/>
+      <c r="J4" s="42"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
       <c r="M4" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N4" s="43"/>
+      <c r="N4" s="44"/>
       <c r="O4" s="23"/>
     </row>
     <row r="5" s="13" customFormat="1" spans="1:15">
@@ -1796,21 +1792,21 @@
         <v>31</v>
       </c>
       <c r="D5" s="25"/>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="41"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="25"/>
-      <c r="J5" s="41"/>
+      <c r="J5" s="42"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
       <c r="M5" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="60"/>
+      <c r="N5" s="44"/>
+      <c r="O5" s="61"/>
     </row>
     <row r="6" s="13" customFormat="1" spans="1:15">
       <c r="A6" s="23" t="s">
@@ -1823,38 +1819,38 @@
         <v>31</v>
       </c>
       <c r="D6" s="25"/>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="42"/>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
       <c r="I6" s="25"/>
-      <c r="J6" s="41"/>
+      <c r="J6" s="42"/>
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="60"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="61"/>
     </row>
     <row r="7" s="13" customFormat="1" spans="1:15">
       <c r="A7" s="23"/>
       <c r="B7" s="27"/>
       <c r="C7" s="25"/>
       <c r="D7" s="25"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="25"/>
-      <c r="J7" s="41"/>
+      <c r="J7" s="42"/>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
       <c r="M7" s="23"/>
-      <c r="N7" s="43"/>
-      <c r="O7" s="60"/>
+      <c r="N7" s="44"/>
+      <c r="O7" s="61"/>
     </row>
     <row r="8" s="13" customFormat="1" spans="1:15">
       <c r="A8" s="23" t="s">
@@ -1867,21 +1863,21 @@
         <v>36</v>
       </c>
       <c r="D8" s="25"/>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="42" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="42"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="25"/>
-      <c r="J8" s="41"/>
+      <c r="J8" s="42"/>
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="60"/>
+      <c r="N8" s="44"/>
+      <c r="O8" s="61"/>
     </row>
     <row r="9" s="13" customFormat="1" spans="1:15">
       <c r="A9" s="30" t="s">
@@ -1896,42 +1892,42 @@
       <c r="D9" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="F9" s="41" t="s">
+      <c r="F9" s="42" t="s">
         <v>42</v>
       </c>
       <c r="G9" s="23"/>
-      <c r="H9" s="43" t="s">
+      <c r="H9" s="44" t="s">
         <v>43</v>
       </c>
       <c r="I9" s="25"/>
-      <c r="J9" s="41"/>
+      <c r="J9" s="42"/>
       <c r="K9" s="23"/>
       <c r="L9" s="23"/>
       <c r="M9" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N9" s="43"/>
-      <c r="O9" s="60"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="61"/>
     </row>
     <row r="10" s="13" customFormat="1" spans="1:15">
       <c r="A10" s="30"/>
       <c r="B10" s="28"/>
       <c r="C10" s="29"/>
       <c r="D10" s="25"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
       <c r="I10" s="25"/>
-      <c r="J10" s="41"/>
+      <c r="J10" s="42"/>
       <c r="K10" s="23"/>
       <c r="L10" s="23"/>
       <c r="M10" s="23"/>
-      <c r="N10" s="43"/>
-      <c r="O10" s="60"/>
+      <c r="N10" s="44"/>
+      <c r="O10" s="61"/>
     </row>
     <row r="11" s="13" customFormat="1" ht="57" spans="1:15">
       <c r="A11" s="30" t="s">
@@ -1944,10 +1940,10 @@
         <v>45</v>
       </c>
       <c r="D11" s="25"/>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="42" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="41"/>
+      <c r="F11" s="42"/>
       <c r="G11" s="23"/>
       <c r="H11" s="23" t="s">
         <v>47</v>
@@ -1955,7 +1951,7 @@
       <c r="I11" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="42" t="s">
         <v>49</v>
       </c>
       <c r="K11" s="23"/>
@@ -1963,188 +1959,189 @@
       <c r="M11" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="N11" s="43"/>
-      <c r="O11" s="60"/>
+      <c r="N11" s="44"/>
+      <c r="O11" s="61"/>
     </row>
     <row r="12" s="13" customFormat="1" spans="1:15">
       <c r="A12" s="30"/>
       <c r="B12" s="28"/>
       <c r="C12" s="29"/>
       <c r="D12" s="25"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="E12" s="42"/>
+      <c r="F12" s="42"/>
       <c r="G12" s="23"/>
       <c r="H12" s="23"/>
       <c r="I12" s="25"/>
-      <c r="J12" s="41"/>
+      <c r="J12" s="42"/>
       <c r="K12" s="23"/>
       <c r="L12" s="23"/>
       <c r="M12" s="23"/>
       <c r="N12" s="23"/>
-      <c r="O12" s="60"/>
+      <c r="O12" s="61"/>
     </row>
     <row r="13" s="13" customFormat="1" spans="1:15">
-      <c r="A13" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>52</v>
-      </c>
+      <c r="A13" s="30"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="25"/>
-      <c r="E13" s="41" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="41"/>
+      <c r="E13" s="42"/>
+      <c r="F13" s="42"/>
       <c r="G13" s="23"/>
       <c r="H13" s="23"/>
       <c r="I13" s="25"/>
-      <c r="J13" s="41"/>
+      <c r="J13" s="42"/>
       <c r="K13" s="23"/>
       <c r="L13" s="23"/>
       <c r="M13" s="23"/>
       <c r="N13" s="23"/>
-      <c r="O13" s="60"/>
+      <c r="O13" s="61"/>
     </row>
     <row r="14" s="13" customFormat="1" spans="1:15">
-      <c r="A14" s="32"/>
-      <c r="B14" s="28"/>
-      <c r="C14" s="33"/>
-      <c r="D14" s="34"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="46"/>
-      <c r="G14" s="47"/>
-      <c r="H14" s="43"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="55"/>
-      <c r="K14" s="47"/>
-      <c r="L14" s="47"/>
-      <c r="M14" s="43"/>
+      <c r="A14" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="48"/>
+      <c r="G14" s="49"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="34"/>
+      <c r="J14" s="47"/>
+      <c r="K14" s="49"/>
+      <c r="L14" s="49"/>
+      <c r="M14" s="44"/>
       <c r="N14" s="23"/>
-      <c r="O14" s="60"/>
+      <c r="O14" s="23"/>
     </row>
     <row r="15" s="13" customFormat="1" spans="1:15">
       <c r="A15" s="8" t="s">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B15" s="35" t="s">
-        <v>54</v>
-      </c>
-      <c r="C15" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="34" t="s">
+      <c r="C15" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E15" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F15" s="46"/>
-      <c r="G15" s="48"/>
+      <c r="E15" s="43" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="50"/>
+      <c r="G15" s="51"/>
       <c r="H15" s="8"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="57"/>
-      <c r="K15" s="48"/>
-      <c r="L15" s="48"/>
-      <c r="M15" s="43" t="s">
+      <c r="I15" s="57"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="L15" s="51"/>
+      <c r="M15" s="44" t="s">
         <v>25</v>
       </c>
       <c r="N15" s="23"/>
-      <c r="O15" s="60"/>
+      <c r="O15" s="61"/>
     </row>
     <row r="16" s="13" customFormat="1" spans="1:15">
-      <c r="A16" s="36"/>
-      <c r="B16" s="36"/>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="49"/>
-      <c r="G16" s="50"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="58"/>
-      <c r="J16" s="59"/>
-      <c r="K16" s="50"/>
-      <c r="L16" s="50"/>
-      <c r="M16" s="36"/>
-      <c r="N16" s="61"/>
-      <c r="O16" s="62"/>
+      <c r="A16" s="37"/>
+      <c r="B16" s="37"/>
+      <c r="C16" s="38"/>
+      <c r="D16" s="39"/>
+      <c r="E16" s="45"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="54"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="37"/>
+      <c r="N16" s="62"/>
+      <c r="O16" s="63"/>
     </row>
     <row r="17" spans="1:15">
       <c r="A17" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B17" s="39" t="s">
-        <v>58</v>
-      </c>
-      <c r="C17" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="40" t="s">
+      <c r="B17" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E17" s="52" t="s">
-        <v>60</v>
+      <c r="E17" s="55" t="s">
+        <v>62</v>
       </c>
       <c r="F17" s="11"/>
       <c r="G17" s="9"/>
-      <c r="H17" s="39"/>
+      <c r="H17" s="40"/>
       <c r="I17" s="10"/>
       <c r="J17" s="11"/>
-      <c r="K17" s="48"/>
+      <c r="K17" s="51"/>
       <c r="L17" s="9"/>
-      <c r="M17" s="43"/>
+      <c r="M17" s="44"/>
       <c r="N17" s="9"/>
       <c r="O17" s="9"/>
     </row>
     <row r="18" spans="1:15">
       <c r="A18" s="8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="B18" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="52"/>
+      <c r="E18" s="55"/>
       <c r="F18" s="11"/>
       <c r="G18" s="9"/>
-      <c r="H18" s="39"/>
+      <c r="H18" s="40"/>
       <c r="I18" s="10"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="48"/>
+      <c r="K18" s="51"/>
       <c r="L18" s="9"/>
-      <c r="M18" s="43"/>
+      <c r="M18" s="44"/>
       <c r="N18" s="9"/>
       <c r="O18" s="9"/>
     </row>
     <row r="19" spans="1:15">
-      <c r="A19" s="39" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" s="40" t="s">
+      <c r="A19" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="40" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="40" t="s">
+      <c r="D19" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="52"/>
+      <c r="E19" s="55"/>
       <c r="F19" s="11"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="39"/>
+      <c r="H19" s="40"/>
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="48"/>
+      <c r="K19" s="51"/>
       <c r="L19" s="9"/>
-      <c r="M19" s="43"/>
+      <c r="M19" s="44"/>
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
@@ -2163,7 +2160,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -2178,7 +2175,7 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>1</v>
@@ -2190,16 +2187,16 @@
         <v>4</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F1" s="15" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G1" s="16" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H1" s="16" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I1" s="12"/>
     </row>
@@ -2216,116 +2213,116 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="8" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="E4" s="19"/>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -2350,8 +2347,8 @@
   <sheetPr/>
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
@@ -2362,24 +2359,24 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C2" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>